<commit_message>
第十二次提交： samples/s1_demo.py importdata.py 整合excel实战 common/requests_utils.py 添加异常处理
</commit_message>
<xml_diff>
--- a/test_data/test_case.xlsx
+++ b/test_data/test_case.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48">
   <si>
     <t>测试用例编号</t>
   </si>
@@ -88,7 +88,7 @@
     <t>json键是否存在</t>
   </si>
   <si>
-    <t>access_token,expires_in</t>
+    <t>access_token1,expires_in</t>
   </si>
   <si>
     <t>case02</t>
@@ -106,40 +106,43 @@
     <t>token</t>
   </si>
   <si>
+    <t>.access_token</t>
+  </si>
+  <si>
+    <t>正则匹配</t>
+  </si>
+  <si>
+    <t>{"access_token":"(.+?)","expires_in":(.+?)}</t>
+  </si>
+  <si>
+    <t>step_02</t>
+  </si>
+  <si>
+    <t>创建标签接口</t>
+  </si>
+  <si>
+    <t>post</t>
+  </si>
+  <si>
+    <t>/cgi-bin/tags/create</t>
+  </si>
+  <si>
+    <t>{"access_token":${token}}</t>
+  </si>
+  <si>
+    <t>{"tag" : {"name" : "衡东8888"}}</t>
+  </si>
+  <si>
+    <t>{"tag":{"id":(.+?),"name":"衡东8888"}}</t>
+  </si>
+  <si>
+    <t>case03</t>
+  </si>
+  <si>
+    <t>测试能否正确删除用户标签</t>
+  </si>
+  <si>
     <t>$.access_token</t>
-  </si>
-  <si>
-    <t>正则匹配</t>
-  </si>
-  <si>
-    <t>{"access_token":"(.+?)","expires_in":(.+?)}</t>
-  </si>
-  <si>
-    <t>step_02</t>
-  </si>
-  <si>
-    <t>创建标签接口</t>
-  </si>
-  <si>
-    <t>post</t>
-  </si>
-  <si>
-    <t>/cgi-bin/tags/create</t>
-  </si>
-  <si>
-    <t>{"access_token":${token}}</t>
-  </si>
-  <si>
-    <t>{"tag" : {"name" : "衡东8888"}}</t>
-  </si>
-  <si>
-    <t>{"tag":{"id":(.+?),"name":"衡东8888"}}</t>
-  </si>
-  <si>
-    <t>case03</t>
-  </si>
-  <si>
-    <t>测试能否正确删除用户标签</t>
   </si>
   <si>
     <t>删除标签接口</t>
@@ -184,6 +187,13 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="宋体"/>
       <charset val="0"/>
@@ -199,22 +209,30 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="11"/>
+      <sz val="13"/>
       <color theme="3"/>
       <name val="宋体"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -228,25 +246,17 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <i/>
       <sz val="11"/>
       <color rgb="FF7F7F7F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -262,7 +272,14 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -270,7 +287,37 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -280,50 +327,6 @@
       <color rgb="FF9C6500"/>
       <name val="宋体"/>
       <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -342,19 +345,157 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
+        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -366,157 +507,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -530,32 +533,11 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -619,11 +601,32 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -632,148 +635,148 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="17" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="10" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="24" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="13" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="10" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="14" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="7" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1106,7 +1109,7 @@
   <dimension ref="A1:N8"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="176" zoomScaleNormal="176" topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="J3" sqref="J3"/>
+      <selection activeCell="K4" sqref="K4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="17.6" outlineLevelRow="7"/>
@@ -1308,7 +1311,7 @@
         <v>29</v>
       </c>
       <c r="L5" t="s">
-        <v>30</v>
+        <v>42</v>
       </c>
       <c r="M5" t="s">
         <v>31</v>
@@ -1322,28 +1325,28 @@
         <v>33</v>
       </c>
       <c r="E6" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="F6" t="s">
         <v>35</v>
       </c>
       <c r="G6" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="H6" t="s">
         <v>37</v>
       </c>
       <c r="I6" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="J6" t="s">
         <v>22</v>
       </c>
       <c r="M6" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="N6" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="8" ht="28.8" spans="8:8">

</xml_diff>

<commit_message>
第十三次提交： api_testcases/api_test.py 编辑测试用例 common/testdata_utils.py 把case_name改为case_id
</commit_message>
<xml_diff>
--- a/test_data/test_case.xlsx
+++ b/test_data/test_case.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47">
   <si>
     <t>测试用例编号</t>
   </si>
@@ -88,7 +88,7 @@
     <t>json键是否存在</t>
   </si>
   <si>
-    <t>access_token1,expires_in</t>
+    <t>access_token,expires_in</t>
   </si>
   <si>
     <t>case02</t>
@@ -106,7 +106,7 @@
     <t>token</t>
   </si>
   <si>
-    <t>.access_token</t>
+    <t>$.access_token</t>
   </si>
   <si>
     <t>正则匹配</t>
@@ -133,16 +133,13 @@
     <t>{"tag" : {"name" : "衡东8888"}}</t>
   </si>
   <si>
-    <t>{"tag":{"id":(.+?),"name":"衡东8888"}}</t>
+    <t>{"tag":{"id":(.+?),"name":"sss"}}</t>
   </si>
   <si>
     <t>case03</t>
   </si>
   <si>
     <t>测试能否正确删除用户标签</t>
-  </si>
-  <si>
-    <t>$.access_token</t>
   </si>
   <si>
     <t>删除标签接口</t>
@@ -1108,8 +1105,8 @@
   <sheetPr/>
   <dimension ref="A1:N8"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="176" zoomScaleNormal="176" topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="K4" sqref="K4"/>
+    <sheetView tabSelected="1" zoomScale="176" zoomScaleNormal="176" topLeftCell="J2" workbookViewId="0">
+      <selection activeCell="N4" sqref="N4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="17.6" outlineLevelRow="7"/>
@@ -1311,7 +1308,7 @@
         <v>29</v>
       </c>
       <c r="L5" t="s">
-        <v>42</v>
+        <v>30</v>
       </c>
       <c r="M5" t="s">
         <v>31</v>
@@ -1325,28 +1322,28 @@
         <v>33</v>
       </c>
       <c r="E6" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F6" t="s">
         <v>35</v>
       </c>
       <c r="G6" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="H6" t="s">
         <v>37</v>
       </c>
       <c r="I6" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="J6" t="s">
         <v>22</v>
       </c>
       <c r="M6" t="s">
+        <v>45</v>
+      </c>
+      <c r="N6" t="s">
         <v>46</v>
-      </c>
-      <c r="N6" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="8" ht="28.8" spans="8:8">

</xml_diff>

<commit_message>
第十四次提交： common/HTMLTestReportCN.py 网页版报告 common/email_utils.py 邮件功能封装
</commit_message>
<xml_diff>
--- a/test_data/test_case.xlsx
+++ b/test_data/test_case.xlsx
@@ -1105,14 +1105,14 @@
   <sheetPr/>
   <dimension ref="A1:N8"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="176" zoomScaleNormal="176" topLeftCell="J2" workbookViewId="0">
-      <selection activeCell="N4" sqref="N4"/>
+    <sheetView tabSelected="1" zoomScale="176" zoomScaleNormal="176" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3:B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="17.6" outlineLevelRow="7"/>
   <cols>
     <col min="1" max="1" width="14.1339285714286" customWidth="1"/>
-    <col min="2" max="2" width="35.0982142857143" customWidth="1"/>
+    <col min="2" max="2" width="40.5714285714286" customWidth="1"/>
     <col min="3" max="3" width="11.1517857142857" customWidth="1"/>
     <col min="4" max="4" width="16.0178571428571" customWidth="1"/>
     <col min="5" max="5" width="21.2678571428571" customWidth="1"/>

</xml_diff>